<commit_message>
mengganti file template stock
</commit_message>
<xml_diff>
--- a/backend/download/template_stock.xlsx
+++ b/backend/download/template_stock.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Real Project\Store Management\Document\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Navyrine\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CF13B7-80B1-41EF-BABD-A451C73E7074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA9F909-D553-4646-B554-D79C7EB9B15D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>warehouse_name</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>sn</t>
+  </si>
+  <si>
+    <t>barcode</t>
   </si>
 </sst>
 </file>
@@ -101,7 +104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -109,10 +112,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E301"/>
+  <dimension ref="A1:F301"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -404,635 +408,641 @@
     <col min="1" max="2" width="26.08984375" style="2" customWidth="1"/>
     <col min="3" max="3" width="25.90625" style="2" customWidth="1"/>
     <col min="4" max="5" width="26.08984375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.5">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.5">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" s="1"/>
-      <c r="B102" s="4"/>
+      <c r="B102" s="3"/>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A103" s="4"/>
-      <c r="B103" s="4"/>
+      <c r="A103" s="3"/>
+      <c r="B103" s="3"/>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A104" s="4"/>
-      <c r="B104" s="4"/>
+      <c r="A104" s="3"/>
+      <c r="B104" s="3"/>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A105" s="4"/>
-      <c r="B105" s="4"/>
+      <c r="A105" s="3"/>
+      <c r="B105" s="3"/>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A106" s="4"/>
-      <c r="B106" s="4"/>
+      <c r="A106" s="3"/>
+      <c r="B106" s="3"/>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A107" s="4"/>
-      <c r="B107" s="4"/>
+      <c r="A107" s="3"/>
+      <c r="B107" s="3"/>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A108" s="4"/>
-      <c r="B108" s="4"/>
+      <c r="A108" s="3"/>
+      <c r="B108" s="3"/>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A109" s="4"/>
-      <c r="B109" s="4"/>
+      <c r="A109" s="3"/>
+      <c r="B109" s="3"/>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A110" s="4"/>
-      <c r="B110" s="4"/>
+      <c r="A110" s="3"/>
+      <c r="B110" s="3"/>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A111" s="4"/>
-      <c r="B111" s="4"/>
+      <c r="A111" s="3"/>
+      <c r="B111" s="3"/>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A112" s="4"/>
-      <c r="B112" s="4"/>
+      <c r="A112" s="3"/>
+      <c r="B112" s="3"/>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A113" s="4"/>
-      <c r="B113" s="4"/>
+      <c r="A113" s="3"/>
+      <c r="B113" s="3"/>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A114" s="4"/>
-      <c r="B114" s="4"/>
+      <c r="A114" s="3"/>
+      <c r="B114" s="3"/>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A115" s="4"/>
-      <c r="B115" s="4"/>
+      <c r="A115" s="3"/>
+      <c r="B115" s="3"/>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A116" s="4"/>
-      <c r="B116" s="4"/>
+      <c r="A116" s="3"/>
+      <c r="B116" s="3"/>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A117" s="4"/>
-      <c r="B117" s="4"/>
+      <c r="A117" s="3"/>
+      <c r="B117" s="3"/>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A118" s="4"/>
-      <c r="B118" s="4"/>
+      <c r="A118" s="3"/>
+      <c r="B118" s="3"/>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A119" s="4"/>
-      <c r="B119" s="4"/>
+      <c r="A119" s="3"/>
+      <c r="B119" s="3"/>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A120" s="4"/>
-      <c r="B120" s="4"/>
+      <c r="A120" s="3"/>
+      <c r="B120" s="3"/>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A121" s="4"/>
-      <c r="B121" s="4"/>
+      <c r="A121" s="3"/>
+      <c r="B121" s="3"/>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A122" s="4"/>
-      <c r="B122" s="4"/>
+      <c r="A122" s="3"/>
+      <c r="B122" s="3"/>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A123" s="4"/>
-      <c r="B123" s="4"/>
+      <c r="A123" s="3"/>
+      <c r="B123" s="3"/>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A124" s="4"/>
-      <c r="B124" s="4"/>
+      <c r="A124" s="3"/>
+      <c r="B124" s="3"/>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A125" s="4"/>
-      <c r="B125" s="4"/>
+      <c r="A125" s="3"/>
+      <c r="B125" s="3"/>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A126" s="4"/>
-      <c r="B126" s="4"/>
+      <c r="A126" s="3"/>
+      <c r="B126" s="3"/>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A127" s="4"/>
-      <c r="B127" s="4"/>
+      <c r="A127" s="3"/>
+      <c r="B127" s="3"/>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A128" s="4"/>
-      <c r="B128" s="4"/>
+      <c r="A128" s="3"/>
+      <c r="B128" s="3"/>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A129" s="4"/>
-      <c r="B129" s="4"/>
+      <c r="A129" s="3"/>
+      <c r="B129" s="3"/>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A130" s="4"/>
-      <c r="B130" s="4"/>
+      <c r="A130" s="3"/>
+      <c r="B130" s="3"/>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A131" s="4"/>
-      <c r="B131" s="4"/>
+      <c r="A131" s="3"/>
+      <c r="B131" s="3"/>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A132" s="4"/>
-      <c r="B132" s="4"/>
+      <c r="A132" s="3"/>
+      <c r="B132" s="3"/>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A133" s="4"/>
-      <c r="B133" s="4"/>
+      <c r="A133" s="3"/>
+      <c r="B133" s="3"/>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A134" s="4"/>
-      <c r="B134" s="4"/>
+      <c r="A134" s="3"/>
+      <c r="B134" s="3"/>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A135" s="4"/>
-      <c r="B135" s="4"/>
+      <c r="A135" s="3"/>
+      <c r="B135" s="3"/>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A136" s="4"/>
-      <c r="B136" s="4"/>
+      <c r="A136" s="3"/>
+      <c r="B136" s="3"/>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A137" s="4"/>
-      <c r="B137" s="4"/>
+      <c r="A137" s="3"/>
+      <c r="B137" s="3"/>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A138" s="4"/>
-      <c r="B138" s="4"/>
+      <c r="A138" s="3"/>
+      <c r="B138" s="3"/>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A139" s="4"/>
-      <c r="B139" s="4"/>
+      <c r="A139" s="3"/>
+      <c r="B139" s="3"/>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A140" s="4"/>
-      <c r="B140" s="4"/>
+      <c r="A140" s="3"/>
+      <c r="B140" s="3"/>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A141" s="4"/>
-      <c r="B141" s="4"/>
+      <c r="A141" s="3"/>
+      <c r="B141" s="3"/>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A142" s="4"/>
-      <c r="B142" s="4"/>
+      <c r="A142" s="3"/>
+      <c r="B142" s="3"/>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A143" s="4"/>
-      <c r="B143" s="4"/>
+      <c r="A143" s="3"/>
+      <c r="B143" s="3"/>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A144" s="4"/>
-      <c r="B144" s="4"/>
+      <c r="A144" s="3"/>
+      <c r="B144" s="3"/>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A145" s="4"/>
-      <c r="B145" s="4"/>
+      <c r="A145" s="3"/>
+      <c r="B145" s="3"/>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A146" s="4"/>
-      <c r="B146" s="4"/>
+      <c r="A146" s="3"/>
+      <c r="B146" s="3"/>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A147" s="4"/>
-      <c r="B147" s="4"/>
+      <c r="A147" s="3"/>
+      <c r="B147" s="3"/>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A148" s="4"/>
-      <c r="B148" s="4"/>
+      <c r="A148" s="3"/>
+      <c r="B148" s="3"/>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A149" s="4"/>
-      <c r="B149" s="4"/>
+      <c r="A149" s="3"/>
+      <c r="B149" s="3"/>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A150" s="4"/>
-      <c r="B150" s="4"/>
+      <c r="A150" s="3"/>
+      <c r="B150" s="3"/>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A151" s="4"/>
-      <c r="B151" s="4"/>
+      <c r="A151" s="3"/>
+      <c r="B151" s="3"/>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A202" s="1"/>
-      <c r="B202" s="4"/>
+      <c r="B202" s="3"/>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A203" s="4"/>
-      <c r="B203" s="4"/>
+      <c r="A203" s="3"/>
+      <c r="B203" s="3"/>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A204" s="4"/>
-      <c r="B204" s="4"/>
+      <c r="A204" s="3"/>
+      <c r="B204" s="3"/>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A205" s="4"/>
-      <c r="B205" s="4"/>
+      <c r="A205" s="3"/>
+      <c r="B205" s="3"/>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A206" s="4"/>
-      <c r="B206" s="4"/>
+      <c r="A206" s="3"/>
+      <c r="B206" s="3"/>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A207" s="4"/>
-      <c r="B207" s="4"/>
+      <c r="A207" s="3"/>
+      <c r="B207" s="3"/>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A208" s="4"/>
-      <c r="B208" s="4"/>
+      <c r="A208" s="3"/>
+      <c r="B208" s="3"/>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A209" s="4"/>
-      <c r="B209" s="4"/>
+      <c r="A209" s="3"/>
+      <c r="B209" s="3"/>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A210" s="4"/>
-      <c r="B210" s="4"/>
+      <c r="A210" s="3"/>
+      <c r="B210" s="3"/>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A211" s="4"/>
-      <c r="B211" s="4"/>
+      <c r="A211" s="3"/>
+      <c r="B211" s="3"/>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A212" s="4"/>
-      <c r="B212" s="4"/>
+      <c r="A212" s="3"/>
+      <c r="B212" s="3"/>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A213" s="4"/>
-      <c r="B213" s="4"/>
+      <c r="A213" s="3"/>
+      <c r="B213" s="3"/>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A214" s="4"/>
-      <c r="B214" s="4"/>
+      <c r="A214" s="3"/>
+      <c r="B214" s="3"/>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A215" s="4"/>
-      <c r="B215" s="4"/>
+      <c r="A215" s="3"/>
+      <c r="B215" s="3"/>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A216" s="4"/>
-      <c r="B216" s="4"/>
+      <c r="A216" s="3"/>
+      <c r="B216" s="3"/>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A217" s="4"/>
-      <c r="B217" s="4"/>
+      <c r="A217" s="3"/>
+      <c r="B217" s="3"/>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A218" s="4"/>
-      <c r="B218" s="4"/>
+      <c r="A218" s="3"/>
+      <c r="B218" s="3"/>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A219" s="4"/>
-      <c r="B219" s="4"/>
+      <c r="A219" s="3"/>
+      <c r="B219" s="3"/>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A220" s="4"/>
-      <c r="B220" s="4"/>
+      <c r="A220" s="3"/>
+      <c r="B220" s="3"/>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A221" s="4"/>
-      <c r="B221" s="4"/>
+      <c r="A221" s="3"/>
+      <c r="B221" s="3"/>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A222" s="4"/>
-      <c r="B222" s="4"/>
+      <c r="A222" s="3"/>
+      <c r="B222" s="3"/>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A223" s="4"/>
-      <c r="B223" s="4"/>
+      <c r="A223" s="3"/>
+      <c r="B223" s="3"/>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A224" s="4"/>
-      <c r="B224" s="4"/>
+      <c r="A224" s="3"/>
+      <c r="B224" s="3"/>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A225" s="4"/>
-      <c r="B225" s="4"/>
+      <c r="A225" s="3"/>
+      <c r="B225" s="3"/>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A226" s="4"/>
-      <c r="B226" s="4"/>
+      <c r="A226" s="3"/>
+      <c r="B226" s="3"/>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A227" s="4"/>
-      <c r="B227" s="4"/>
+      <c r="A227" s="3"/>
+      <c r="B227" s="3"/>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A228" s="4"/>
-      <c r="B228" s="4"/>
+      <c r="A228" s="3"/>
+      <c r="B228" s="3"/>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A229" s="4"/>
-      <c r="B229" s="4"/>
+      <c r="A229" s="3"/>
+      <c r="B229" s="3"/>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A230" s="4"/>
-      <c r="B230" s="4"/>
+      <c r="A230" s="3"/>
+      <c r="B230" s="3"/>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A231" s="4"/>
-      <c r="B231" s="4"/>
+      <c r="A231" s="3"/>
+      <c r="B231" s="3"/>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A232" s="4"/>
-      <c r="B232" s="4"/>
+      <c r="A232" s="3"/>
+      <c r="B232" s="3"/>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A233" s="4"/>
-      <c r="B233" s="4"/>
+      <c r="A233" s="3"/>
+      <c r="B233" s="3"/>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A234" s="4"/>
-      <c r="B234" s="4"/>
+      <c r="A234" s="3"/>
+      <c r="B234" s="3"/>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A235" s="4"/>
-      <c r="B235" s="4"/>
+      <c r="A235" s="3"/>
+      <c r="B235" s="3"/>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A236" s="4"/>
-      <c r="B236" s="4"/>
+      <c r="A236" s="3"/>
+      <c r="B236" s="3"/>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A237" s="4"/>
-      <c r="B237" s="4"/>
+      <c r="A237" s="3"/>
+      <c r="B237" s="3"/>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A238" s="4"/>
-      <c r="B238" s="4"/>
+      <c r="A238" s="3"/>
+      <c r="B238" s="3"/>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A239" s="4"/>
-      <c r="B239" s="4"/>
+      <c r="A239" s="3"/>
+      <c r="B239" s="3"/>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A240" s="4"/>
-      <c r="B240" s="4"/>
+      <c r="A240" s="3"/>
+      <c r="B240" s="3"/>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A241" s="4"/>
-      <c r="B241" s="4"/>
+      <c r="A241" s="3"/>
+      <c r="B241" s="3"/>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A242" s="4"/>
-      <c r="B242" s="4"/>
+      <c r="A242" s="3"/>
+      <c r="B242" s="3"/>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A243" s="4"/>
-      <c r="B243" s="4"/>
+      <c r="A243" s="3"/>
+      <c r="B243" s="3"/>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A244" s="4"/>
-      <c r="B244" s="4"/>
+      <c r="A244" s="3"/>
+      <c r="B244" s="3"/>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A245" s="4"/>
-      <c r="B245" s="4"/>
+      <c r="A245" s="3"/>
+      <c r="B245" s="3"/>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A246" s="4"/>
-      <c r="B246" s="4"/>
+      <c r="A246" s="3"/>
+      <c r="B246" s="3"/>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A247" s="4"/>
-      <c r="B247" s="4"/>
+      <c r="A247" s="3"/>
+      <c r="B247" s="3"/>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A248" s="4"/>
-      <c r="B248" s="4"/>
+      <c r="A248" s="3"/>
+      <c r="B248" s="3"/>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A249" s="4"/>
-      <c r="B249" s="4"/>
+      <c r="A249" s="3"/>
+      <c r="B249" s="3"/>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A250" s="4"/>
-      <c r="B250" s="4"/>
+      <c r="A250" s="3"/>
+      <c r="B250" s="3"/>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A251" s="4"/>
-      <c r="B251" s="4"/>
+      <c r="A251" s="3"/>
+      <c r="B251" s="3"/>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A252" s="4"/>
-      <c r="B252" s="4"/>
+      <c r="A252" s="3"/>
+      <c r="B252" s="3"/>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A253" s="4"/>
-      <c r="B253" s="4"/>
+      <c r="A253" s="3"/>
+      <c r="B253" s="3"/>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A254" s="4"/>
-      <c r="B254" s="4"/>
+      <c r="A254" s="3"/>
+      <c r="B254" s="3"/>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A255" s="4"/>
-      <c r="B255" s="4"/>
+      <c r="A255" s="3"/>
+      <c r="B255" s="3"/>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A256" s="4"/>
-      <c r="B256" s="4"/>
+      <c r="A256" s="3"/>
+      <c r="B256" s="3"/>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A257" s="4"/>
-      <c r="B257" s="4"/>
+      <c r="A257" s="3"/>
+      <c r="B257" s="3"/>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A258" s="4"/>
-      <c r="B258" s="4"/>
+      <c r="A258" s="3"/>
+      <c r="B258" s="3"/>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A259" s="4"/>
-      <c r="B259" s="4"/>
+      <c r="A259" s="3"/>
+      <c r="B259" s="3"/>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A260" s="4"/>
-      <c r="B260" s="4"/>
+      <c r="A260" s="3"/>
+      <c r="B260" s="3"/>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A261" s="4"/>
-      <c r="B261" s="4"/>
+      <c r="A261" s="3"/>
+      <c r="B261" s="3"/>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A262" s="4"/>
-      <c r="B262" s="4"/>
+      <c r="A262" s="3"/>
+      <c r="B262" s="3"/>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A263" s="4"/>
-      <c r="B263" s="4"/>
+      <c r="A263" s="3"/>
+      <c r="B263" s="3"/>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A264" s="4"/>
-      <c r="B264" s="4"/>
+      <c r="A264" s="3"/>
+      <c r="B264" s="3"/>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A265" s="4"/>
-      <c r="B265" s="4"/>
+      <c r="A265" s="3"/>
+      <c r="B265" s="3"/>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A266" s="4"/>
-      <c r="B266" s="4"/>
+      <c r="A266" s="3"/>
+      <c r="B266" s="3"/>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A267" s="4"/>
-      <c r="B267" s="4"/>
+      <c r="A267" s="3"/>
+      <c r="B267" s="3"/>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A268" s="4"/>
-      <c r="B268" s="4"/>
+      <c r="A268" s="3"/>
+      <c r="B268" s="3"/>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A269" s="4"/>
-      <c r="B269" s="4"/>
+      <c r="A269" s="3"/>
+      <c r="B269" s="3"/>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A270" s="4"/>
-      <c r="B270" s="4"/>
+      <c r="A270" s="3"/>
+      <c r="B270" s="3"/>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A271" s="4"/>
-      <c r="B271" s="4"/>
+      <c r="A271" s="3"/>
+      <c r="B271" s="3"/>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A272" s="4"/>
-      <c r="B272" s="4"/>
+      <c r="A272" s="3"/>
+      <c r="B272" s="3"/>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A273" s="4"/>
-      <c r="B273" s="4"/>
+      <c r="A273" s="3"/>
+      <c r="B273" s="3"/>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A274" s="4"/>
-      <c r="B274" s="4"/>
+      <c r="A274" s="3"/>
+      <c r="B274" s="3"/>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A275" s="4"/>
-      <c r="B275" s="4"/>
+      <c r="A275" s="3"/>
+      <c r="B275" s="3"/>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A276" s="4"/>
-      <c r="B276" s="4"/>
+      <c r="A276" s="3"/>
+      <c r="B276" s="3"/>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A277" s="4"/>
-      <c r="B277" s="4"/>
+      <c r="A277" s="3"/>
+      <c r="B277" s="3"/>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A278" s="4"/>
-      <c r="B278" s="4"/>
+      <c r="A278" s="3"/>
+      <c r="B278" s="3"/>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A279" s="4"/>
-      <c r="B279" s="4"/>
+      <c r="A279" s="3"/>
+      <c r="B279" s="3"/>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A280" s="4"/>
-      <c r="B280" s="4"/>
+      <c r="A280" s="3"/>
+      <c r="B280" s="3"/>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A281" s="4"/>
-      <c r="B281" s="4"/>
+      <c r="A281" s="3"/>
+      <c r="B281" s="3"/>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A282" s="4"/>
-      <c r="B282" s="4"/>
+      <c r="A282" s="3"/>
+      <c r="B282" s="3"/>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A283" s="4"/>
-      <c r="B283" s="4"/>
+      <c r="A283" s="3"/>
+      <c r="B283" s="3"/>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A284" s="4"/>
-      <c r="B284" s="4"/>
+      <c r="A284" s="3"/>
+      <c r="B284" s="3"/>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A285" s="4"/>
-      <c r="B285" s="4"/>
+      <c r="A285" s="3"/>
+      <c r="B285" s="3"/>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A286" s="4"/>
-      <c r="B286" s="4"/>
+      <c r="A286" s="3"/>
+      <c r="B286" s="3"/>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A287" s="4"/>
-      <c r="B287" s="4"/>
+      <c r="A287" s="3"/>
+      <c r="B287" s="3"/>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A288" s="4"/>
-      <c r="B288" s="4"/>
+      <c r="A288" s="3"/>
+      <c r="B288" s="3"/>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A289" s="4"/>
-      <c r="B289" s="4"/>
+      <c r="A289" s="3"/>
+      <c r="B289" s="3"/>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A290" s="4"/>
-      <c r="B290" s="4"/>
+      <c r="A290" s="3"/>
+      <c r="B290" s="3"/>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A291" s="4"/>
-      <c r="B291" s="4"/>
+      <c r="A291" s="3"/>
+      <c r="B291" s="3"/>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A292" s="4"/>
-      <c r="B292" s="4"/>
+      <c r="A292" s="3"/>
+      <c r="B292" s="3"/>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A293" s="4"/>
-      <c r="B293" s="4"/>
+      <c r="A293" s="3"/>
+      <c r="B293" s="3"/>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A294" s="4"/>
-      <c r="B294" s="4"/>
+      <c r="A294" s="3"/>
+      <c r="B294" s="3"/>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A295" s="4"/>
-      <c r="B295" s="4"/>
+      <c r="A295" s="3"/>
+      <c r="B295" s="3"/>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A296" s="4"/>
-      <c r="B296" s="4"/>
+      <c r="A296" s="3"/>
+      <c r="B296" s="3"/>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A297" s="4"/>
-      <c r="B297" s="4"/>
+      <c r="A297" s="3"/>
+      <c r="B297" s="3"/>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A298" s="4"/>
-      <c r="B298" s="4"/>
+      <c r="A298" s="3"/>
+      <c r="B298" s="3"/>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A299" s="4"/>
-      <c r="B299" s="4"/>
+      <c r="A299" s="3"/>
+      <c r="B299" s="3"/>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A300" s="4"/>
-      <c r="B300" s="4"/>
+      <c r="A300" s="3"/>
+      <c r="B300" s="3"/>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A301" s="4"/>
-      <c r="B301" s="4"/>
+      <c r="A301" s="3"/>
+      <c r="B301" s="3"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="2ZkVfG9jIc84J1GrV/QXOPbyS69lxu+1WSOnvzmZxubJ2TIlhsAzQfbMvzOOrLezWYYL4jKHuLdF29105090gw==" saltValue="aHOD92PmxsplROF1JdLzxw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="vXO4HBiyxZgDZj/g/vpy2eq5347+qOTTDQWLo5pj2gvFsGmWSgY3LUIjT9ifeBXuQTA3bQxx+t0NKfbVxsssfA==" saltValue="jl1cpdA9t7mIZNKrZLz+LA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ERROR" error="DATA HARUS TEXT" sqref="A302:A1048576 B1:B101 A1:A101 A152:A201 B152:B201 B302:B1048576" xr:uid="{CFDA9269-D8DD-488C-82C9-28BB5A4D43C7}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ERROR" error="DATA HARUS TEXT" sqref="A152:B201 A302:B1048576 A1:B51 A53:B101" xr:uid="{CFDA9269-D8DD-488C-82C9-28BB5A4D43C7}">
       <formula1>ISERROR(VALUE(A1))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>